<commit_message>
typewriter => release branch refresh
</commit_message>
<xml_diff>
--- a/excel/base.xlsx
+++ b/excel/base.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>lowercase</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -358,6 +358,14 @@
   </si>
   <si>
     <t>—</t>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -727,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -766,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -780,7 +788,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -794,7 +802,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -808,7 +816,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -822,7 +830,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -836,7 +844,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -850,7 +858,7 @@
         <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -864,7 +872,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -878,7 +886,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -892,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -903,7 +911,7 @@
         <v>38</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -914,7 +922,7 @@
         <v>39</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -925,7 +933,7 @@
         <v>40</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -936,7 +944,7 @@
         <v>41</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -947,7 +955,7 @@
         <v>42</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -957,8 +965,8 @@
       <c r="C17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>83</v>
+      <c r="G17" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -969,7 +977,7 @@
         <v>44</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -979,8 +987,8 @@
       <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>76</v>
+      <c r="G19" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -991,7 +999,7 @@
         <v>46</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1002,7 +1010,7 @@
         <v>47</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1012,8 +1020,8 @@
       <c r="C22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>85</v>
+      <c r="G22" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1024,7 +1032,7 @@
         <v>49</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1034,8 +1042,8 @@
       <c r="C24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>66</v>
+      <c r="G24" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1046,7 +1054,7 @@
         <v>51</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1057,7 +1065,7 @@
         <v>52</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1068,27 +1076,37 @@
         <v>53</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="14.25">
       <c r="G28" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8">
       <c r="G29" s="1" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="G30" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="G31" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="G32" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7">
+      <c r="G33" s="1" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>